<commit_message>
adding a module that works with csv files
</commit_message>
<xml_diff>
--- a/shoes.xlsx
+++ b/shoes.xlsx
@@ -214,120 +214,120 @@
     <t>Nike Free Run 2 'Triple Black'</t>
   </si>
   <si>
+    <t>Nike React Element 87 'Anthracite'</t>
+  </si>
+  <si>
+    <t>Nike React Element 55 'Triple Black'</t>
+  </si>
+  <si>
+    <t>Nike React Element 55 'Reverse Schematic - Black'</t>
+  </si>
+  <si>
+    <t>Nike React Element 87 'Solar Red'</t>
+  </si>
+  <si>
+    <t>Nike SB Dunk Low Racing Buggy</t>
+  </si>
+  <si>
+    <t>Nike SB Dunk Low x NBA Kobe Bryant</t>
+  </si>
+  <si>
+    <t>Nike SB Dunk Low Travis Scott x Play Station 5 'Khakki'</t>
+  </si>
+  <si>
+    <t>DC Shoes Court Graffik 'White &amp; Black'</t>
+  </si>
+  <si>
+    <t>Nike Air Max 95 Sneaker Boot 'Triple Black'</t>
+  </si>
+  <si>
+    <t>Nike ACG Mountain Fly GTX 'Black'</t>
+  </si>
+  <si>
+    <t>DVS Comanche Grey/White/Yellow/Black</t>
+  </si>
+  <si>
+    <t>Nike Air Jordan 1 mid x Kaws 'Black'</t>
+  </si>
+  <si>
+    <t>Nike Dunk Low Pro SB 'Purple Pigeon'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nike Air Max 95 x CORTEIZ 'Gutta Green' </t>
+  </si>
+  <si>
+    <t>Nike React Vision 'Smoke Grey Orange'</t>
+  </si>
+  <si>
+    <t>Nike React Vision 'Triple Black'</t>
+  </si>
+  <si>
+    <t>DC Shoes Manteca 4 x 'Slayer'</t>
+  </si>
+  <si>
+    <t>Nike P-6000 'Athletic Department'</t>
+  </si>
+  <si>
+    <t>Superstar 'Core Black/White'</t>
+  </si>
+  <si>
+    <t>DC Stag 'black/orange'</t>
+  </si>
+  <si>
+    <t>DC Stag 'Black/White'</t>
+  </si>
+  <si>
+    <t>DC Stag 'Black/Red'</t>
+  </si>
+  <si>
+    <t>NIKE Air Force 1 Wild 'black'</t>
+  </si>
+  <si>
+    <t>ASICS Gel-Kahana 8 'Black'</t>
+  </si>
+  <si>
+    <t>Converse Run Star Motion 'Black Gum Honey'</t>
+  </si>
+  <si>
+    <t>Forum 84 Low Shoes 'Blue Denim Gum'</t>
+  </si>
+  <si>
+    <t>Converse X COMME Des GARCONS PLAY Chuck 70 Hi 'Black Red'</t>
+  </si>
+  <si>
+    <t>Nike Air Max 90 Essential 'Hyper Jade'</t>
+  </si>
+  <si>
+    <t>Yeezy Boost 350 V2 'Desert Sage'</t>
+  </si>
+  <si>
+    <t>yeezy 350 v2 grey orange</t>
+  </si>
+  <si>
+    <t>Nike Air Zoom Pegasus 39 'Black White'</t>
+  </si>
+  <si>
+    <t>Nike Air Zoom Pegasus 39 TB 'White Black'</t>
+  </si>
+  <si>
+    <t>Birkenstock Chocolate</t>
+  </si>
+  <si>
+    <t>Nike React Vision 'Wolf Grey'</t>
+  </si>
+  <si>
+    <t>Nike React Vision 'White'</t>
+  </si>
+  <si>
+    <t>ASICS Gel-Kayano 14 'Ironclad Cloud Grey'</t>
+  </si>
+  <si>
+    <t>ASICS Gel Quantum Kinetic 'Dark Sepia Shamrock'</t>
+  </si>
+  <si>
     <t>Nike Air Max 95 'Neutral Olive'</t>
   </si>
   <si>
-    <t>Nike React Element 87 'Anthracite'</t>
-  </si>
-  <si>
-    <t>Nike React Element 55 'Triple Black'</t>
-  </si>
-  <si>
-    <t>Nike React Element 55 'Reverse Schematic - Black'</t>
-  </si>
-  <si>
-    <t>Nike React Element 87 'Solar Red'</t>
-  </si>
-  <si>
-    <t>Nike SB Dunk Low Racing Buggy</t>
-  </si>
-  <si>
-    <t>Nike SB Dunk Low x NBA Kobe Bryant</t>
-  </si>
-  <si>
-    <t>Nike SB Dunk Low Travis Scott x Play Station 5 'Khakki'</t>
-  </si>
-  <si>
-    <t>DC Shoes Court Graffik 'White &amp; Black'</t>
-  </si>
-  <si>
-    <t>Nike Air Max 95 Sneaker Boot 'Triple Black'</t>
-  </si>
-  <si>
-    <t>Nike ACG Mountain Fly GTX 'Black'</t>
-  </si>
-  <si>
-    <t>DVS Comanche Grey/White/Yellow/Black</t>
-  </si>
-  <si>
-    <t>Nike Air Jordan 1 mid x Kaws 'Black'</t>
-  </si>
-  <si>
-    <t>Nike Dunk Low Pro SB 'Purple Pigeon'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nike Air Max 95 x CORTEIZ 'Gutta Green' </t>
-  </si>
-  <si>
-    <t>Nike React Vision 'Smoke Grey Orange'</t>
-  </si>
-  <si>
-    <t>Nike React Vision 'Triple Black'</t>
-  </si>
-  <si>
-    <t>DC Shoes Manteca 4 x 'Slayer'</t>
-  </si>
-  <si>
-    <t>Nike P-6000 'Athletic Department'</t>
-  </si>
-  <si>
-    <t>Superstar 'Core Black/White'</t>
-  </si>
-  <si>
-    <t>DC Stag 'black/orange'</t>
-  </si>
-  <si>
-    <t>DC Stag 'Black/White'</t>
-  </si>
-  <si>
-    <t>DC Stag 'Black/Red'</t>
-  </si>
-  <si>
-    <t>NIKE Air Force 1 Wild 'black'</t>
-  </si>
-  <si>
-    <t>ASICS Gel-Kahana 8 'Black'</t>
-  </si>
-  <si>
-    <t>Converse Run Star Motion 'Black Gum Honey'</t>
-  </si>
-  <si>
-    <t>Forum 84 Low Shoes 'Blue Denim Gum'</t>
-  </si>
-  <si>
-    <t>Converse X COMME Des GARCONS PLAY Chuck 70 Hi 'Black Red'</t>
-  </si>
-  <si>
-    <t>Nike Air Max 90 Essential 'Hyper Jade'</t>
-  </si>
-  <si>
-    <t>Yeezy Boost 350 V2 'Desert Sage'</t>
-  </si>
-  <si>
-    <t>yeezy 350 v2 grey orange</t>
-  </si>
-  <si>
-    <t>Nike Air Zoom Pegasus 39 'Black White'</t>
-  </si>
-  <si>
-    <t>Nike Air Zoom Pegasus 39 TB 'White Black'</t>
-  </si>
-  <si>
-    <t>Birkenstock Chocolate</t>
-  </si>
-  <si>
-    <t>Nike React Vision 'Wolf Grey'</t>
-  </si>
-  <si>
-    <t>Nike React Vision 'White'</t>
-  </si>
-  <si>
-    <t>ASICS Gel-Kayano 14 'Ironclad Cloud Grey'</t>
-  </si>
-  <si>
-    <t>ASICS Gel Quantum Kinetic 'Dark Sepia Shamrock'</t>
-  </si>
-  <si>
     <t>Nike Air Max 95 Essential 'Halloween'</t>
   </si>
   <si>
@@ -436,337 +436,337 @@
     <t>Nike Air Max 90 'University Gold'</t>
   </si>
   <si>
+    <t>Nike Air Max 95 Essential 'Armory Navy'</t>
+  </si>
+  <si>
+    <t>Nike x Stash Air Max 95 'Obsidian Black'</t>
+  </si>
+  <si>
+    <t>Campus X Bad Bunny 'Grey'</t>
+  </si>
+  <si>
+    <t>Nike Shox TL 'Sunrise Gradient'</t>
+  </si>
+  <si>
+    <t>ASICS Gel-Nimbus 10.1 'Black Grand Shark'</t>
+  </si>
+  <si>
+    <t>SL 72 OG 'Preloved Brown Almost Yellow'</t>
+  </si>
+  <si>
+    <t>Nike Air Max 95 'Black Grape'</t>
+  </si>
+  <si>
+    <t>Mizuno Adventure Twe</t>
+  </si>
+  <si>
+    <t>Nike Air Max 95 'Topographic'</t>
+  </si>
+  <si>
+    <t>Nike x size? Air Max Dn 'Platinum Violet'</t>
+  </si>
+  <si>
+    <t>Nike Air Max Tailwind 4 'Grey'</t>
+  </si>
+  <si>
+    <t>Saucony Jazz Original Vintage 'Black/White'</t>
+  </si>
+  <si>
+    <t>Nike React Element 55 'Tour Yellow'</t>
+  </si>
+  <si>
+    <t>Nike Kyrie 7 EP 'Midnight Navy'</t>
+  </si>
+  <si>
+    <t>Salomon XT 6 GTX 'Utility Gray'</t>
+  </si>
+  <si>
+    <t>Fear of God Athletics Basketball 'Carbon'</t>
+  </si>
+  <si>
+    <t>Salomon XT-6 Series GTX 'Blue' GORE-TEX</t>
+  </si>
+  <si>
+    <t>DVS Comanche Black/White</t>
+  </si>
+  <si>
+    <t>Air Jordan 1 High "TEATHER Brown&amp;Green&amp; Beige"</t>
+  </si>
+  <si>
+    <t>Nike Air Max Plus Drift 'Bright Crimson Field/Purple'</t>
+  </si>
+  <si>
+    <t>Nike React Vision 'White Anthracite'</t>
+  </si>
+  <si>
+    <t>Nike React Vision 'Black'</t>
+  </si>
+  <si>
+    <t>Handball Spezial 'Core Black/Grey Four'</t>
+  </si>
+  <si>
+    <t>Nike ZoomX Zegama Trail 2 'Daybrake Clay'</t>
+  </si>
+  <si>
+    <t>Ozmillen 'Grey two/ Crystall white'</t>
+  </si>
+  <si>
+    <t>Handball Spezial 'Pantone/Collegiate Navy/Gum'</t>
+  </si>
+  <si>
+    <t>Handball Spezial 'Exclusive Mesh Purple'</t>
+  </si>
+  <si>
+    <t>Yeezy Boost 350 V2 'Ash Pearl'</t>
+  </si>
+  <si>
+    <t>DC SHOES COURT GRAFFIK 'BASQ CT'</t>
+  </si>
+  <si>
+    <t>DC Shoes Court Graffik 'Black/Red'</t>
+  </si>
+  <si>
+    <t>Zig Kinetica 2 Edge GTX 'Black Midnight Pine'</t>
+  </si>
+  <si>
+    <t>NIKE JORDAN 1 MID x Travis Scott 'BLACK PHANTOM'</t>
+  </si>
+  <si>
+    <t>Nike x Off-White Air Rubber Dunk 'Green Strike'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Samba Team x Real Madrid 'White Gum' </t>
+  </si>
+  <si>
+    <t>Nike ZoomX Zegama Trail 'Volt'</t>
+  </si>
+  <si>
+    <t>Campus 00s 'Black/White'</t>
+  </si>
+  <si>
+    <t>Oztral 'Aluminium Grey'</t>
+  </si>
+  <si>
+    <t>Handball Spezial 'Navy Gum'</t>
+  </si>
+  <si>
+    <t>Asics Gel-Kahana 8 'Grey/Blue'</t>
+  </si>
+  <si>
+    <t>Saucony Layer 'Black'</t>
+  </si>
+  <si>
+    <t>ASICS Gel Kayano 14 'Vanilla Tarmac'</t>
+  </si>
+  <si>
+    <t>Nike Air Jordan 4 Retro 'Canyon Purple'</t>
+  </si>
+  <si>
+    <t>Nike Air Max 90 Terrascape 'Sail Sea Glass'</t>
+  </si>
+  <si>
+    <t>Nike X Grateful Dead SB Dunk Low 'Orange Bear'</t>
+  </si>
+  <si>
+    <t>Niteball 'Black Sub Green'</t>
+  </si>
+  <si>
+    <t>Nike Air Jordan 4 Retro SE 'Neon 95'</t>
+  </si>
+  <si>
+    <t>Superstar 'White/Black'</t>
+  </si>
+  <si>
+    <t>Merrell ice cap moc 'black/orange'</t>
+  </si>
+  <si>
+    <t>ASICS Gel-NYC 'Mauve Blue'</t>
+  </si>
+  <si>
     <t xml:space="preserve">Handball Spezial Moscow </t>
   </si>
   <si>
-    <t>Nike Air Max 95 Essential 'Armory Navy'</t>
-  </si>
-  <si>
-    <t>Nike x Stash Air Max 95 'Obsidian Black'</t>
-  </si>
-  <si>
-    <t>Campus X Bad Bunny 'Grey'</t>
-  </si>
-  <si>
-    <t>Nike Shox TL 'Sunrise Gradient'</t>
-  </si>
-  <si>
-    <t>ASICS Gel-Nimbus 10.1 'Black Grand Shark'</t>
-  </si>
-  <si>
-    <t>SL 72 OG 'Preloved Brown Almost Yellow'</t>
-  </si>
-  <si>
-    <t>Nike Air Max 95 'Black Grape'</t>
+    <t>Nike Air Max 95 'Koi'</t>
+  </si>
+  <si>
+    <t>Nike x Supreme Shox Ride 2 SP White/Grey/Volt</t>
+  </si>
+  <si>
+    <t>Nike Air Max 95 Petek 'Dark Blue/Purple'</t>
+  </si>
+  <si>
+    <t>Nike Air Max 95 white/black/fiol</t>
+  </si>
+  <si>
+    <t>Nike Shox Ride 2 'Baroque Brown Diffused Blue</t>
+  </si>
+  <si>
+    <t>Nike Shox TL 'Persian Violet'</t>
+  </si>
+  <si>
+    <t>Nike Nocta Glide Drake 'Khaki'</t>
   </si>
   <si>
     <t xml:space="preserve"> Nike Air Portal x SUPREME 'White/Blue'</t>
   </si>
   <si>
-    <t>Mizuno Adventure Twe</t>
-  </si>
-  <si>
-    <t>Nike Air Max 95 'Topographic'</t>
-  </si>
-  <si>
-    <t>Nike x size? Air Max Dn 'Platinum Violet'</t>
-  </si>
-  <si>
-    <t>Nike Air Max Tailwind 4 'Grey'</t>
-  </si>
-  <si>
-    <t>Saucony Jazz Original Vintage 'Black/White'</t>
-  </si>
-  <si>
-    <t>Nike React Element 55 'Tour Yellow'</t>
-  </si>
-  <si>
-    <t>Nike Kyrie 7 EP 'Midnight Navy'</t>
-  </si>
-  <si>
-    <t>Salomon XT 6 GTX 'Utility Gray'</t>
-  </si>
-  <si>
-    <t>Fear of God Athletics Basketball 'Carbon'</t>
-  </si>
-  <si>
-    <t>Salomon XT-6 Series GTX 'Blue' GORE-TEX</t>
-  </si>
-  <si>
-    <t>DVS Comanche Black/White</t>
-  </si>
-  <si>
-    <t>Air Jordan 1 High "TEATHER Brown&amp;Green&amp; Beige"</t>
-  </si>
-  <si>
-    <t>Nike Air Max Plus Drift 'Bright Crimson Field/Purple'</t>
-  </si>
-  <si>
-    <t>Nike React Vision 'White Anthracite'</t>
-  </si>
-  <si>
-    <t>Nike React Vision 'Black'</t>
-  </si>
-  <si>
-    <t>Handball Spezial 'Core Black/Grey Four'</t>
-  </si>
-  <si>
-    <t>Nike ZoomX Zegama Trail 2 'Daybrake Clay'</t>
-  </si>
-  <si>
-    <t>Ozmillen 'Grey two/ Crystall white'</t>
-  </si>
-  <si>
-    <t>Handball Spezial 'Pantone/Collegiate Navy/Gum'</t>
-  </si>
-  <si>
-    <t>Handball Spezial 'Exclusive Mesh Purple'</t>
-  </si>
-  <si>
-    <t>Yeezy Boost 350 V2 'Ash Pearl'</t>
-  </si>
-  <si>
-    <t>DC SHOES COURT GRAFFIK 'BASQ CT'</t>
-  </si>
-  <si>
-    <t>DC Shoes Court Graffik 'Black/Red'</t>
-  </si>
-  <si>
-    <t>Zig Kinetica 2 Edge GTX 'Black Midnight Pine'</t>
-  </si>
-  <si>
-    <t>NIKE JORDAN 1 MID x Travis Scott 'BLACK PHANTOM'</t>
-  </si>
-  <si>
-    <t>Nike x Off-White Air Rubber Dunk 'Green Strike'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Samba Team x Real Madrid 'White Gum' </t>
-  </si>
-  <si>
-    <t>Nike ZoomX Zegama Trail 'Volt'</t>
-  </si>
-  <si>
-    <t>Campus 00s 'Black/White'</t>
-  </si>
-  <si>
-    <t>Oztral 'Aluminium Grey'</t>
-  </si>
-  <si>
-    <t>Handball Spezial 'Navy Gum'</t>
-  </si>
-  <si>
-    <t>Asics Gel-Kahana 8 'Grey/Blue'</t>
-  </si>
-  <si>
-    <t>Saucony Layer 'Black'</t>
-  </si>
-  <si>
-    <t>ASICS Gel Kayano 14 'Vanilla Tarmac'</t>
-  </si>
-  <si>
-    <t>Nike Air Jordan 4 Retro 'Canyon Purple'</t>
+    <t>Nike Air Max Portal 'Black/White'</t>
+  </si>
+  <si>
+    <t>Nike Air Max 96 'Triple Black'</t>
+  </si>
+  <si>
+    <t>Nike Air Force low 'Venom'</t>
+  </si>
+  <si>
+    <t>Nike Dunk Low 'Year of the Dragon'</t>
+  </si>
+  <si>
+    <t>Nike Kyrie 7 EP 'Chinese New Year'</t>
+  </si>
+  <si>
+    <t>Asics Gel-NYC Gore-Tex 'Black/Bronze'</t>
+  </si>
+  <si>
+    <t>Salomon XT-6 GORE-TEX  'Triple Black'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASICS Gel Kayano Trainer 21 'Black' </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SALOMON XT-6 'Pewter Black Aurora Red' </t>
+  </si>
+  <si>
+    <t>Nike Dunk Low 'Sanddrift Light Armory Blue'</t>
+  </si>
+  <si>
+    <t>Nike Air Jordan 4 retro 'military brown'</t>
+  </si>
+  <si>
+    <t>ASICS Gel-Kayano Trainer 21 'Smoke Blue'</t>
+  </si>
+  <si>
+    <t>Nike Air Max Terrascape Plus 'Triple Black'</t>
+  </si>
+  <si>
+    <t>Salomon XT-6 Series 'Black/Lunar Rock'</t>
+  </si>
+  <si>
+    <t>Globe Tilt trainers 'Dark Shadow/Phantom'</t>
+  </si>
+  <si>
+    <t>DC Shoes Spectre x NEEDLES 'Black/Purple'</t>
+  </si>
+  <si>
+    <t>Iniki Runner 'Core Black 2.0'</t>
+  </si>
+  <si>
+    <t>ASICS Gel 1090 'Silver'</t>
+  </si>
+  <si>
+    <t>Nike Air Zoom Pegasus 38 'Wolf Grey'</t>
+  </si>
+  <si>
+    <t>Nike Zoom Pegasus 39 'Ashen Slate Football Grey Cobalt Bliss'</t>
+  </si>
+  <si>
+    <t>Nike ZoomX Zegama Trail 2 'Black/White'</t>
+  </si>
+  <si>
+    <t>ASICS GEL-1130 X HAL STUDIOS 'Smoke Grey'</t>
+  </si>
+  <si>
+    <t>Nike v2k run 'metallic silver/white'</t>
+  </si>
+  <si>
+    <t>Asics Gel-1130 'Slate Grey/Piedmont Grey'</t>
+  </si>
+  <si>
+    <t>Asics gel-1130 X HAL STUDIOS  'Forest'</t>
+  </si>
+  <si>
+    <t>Suba Sport black red</t>
+  </si>
+  <si>
+    <t>Intimidation Sports Casual Shoes 'Black Purple'</t>
+  </si>
+  <si>
+    <t>Premiata Mick 'Black'</t>
+  </si>
+  <si>
+    <t>Nike SB Dunk Low Vintage 'Phoenix Suns'</t>
+  </si>
+  <si>
+    <t>ASICS GEL SONOMA 15 White/Dark grey</t>
+  </si>
+  <si>
+    <t>Saucony Jazz Original Vintage 'Light Grey'</t>
+  </si>
+  <si>
+    <t>ASICS Gel-Kahana 8 'Dark Blue Brown' demi</t>
+  </si>
+  <si>
+    <t>Zig Kinetica 2 Edge GTX 'Black'</t>
+  </si>
+  <si>
+    <t>Salomon XT-6 'Triple Black'</t>
+  </si>
+  <si>
+    <t>Nike Air Jordan MVP 678 'Raptors'</t>
+  </si>
+  <si>
+    <t>Nike Air Jordan 6 Retro x Travis Scott 'Olive'</t>
+  </si>
+  <si>
+    <t>Nike SB Dunk Low х Stussy 'BMW M3'</t>
+  </si>
+  <si>
+    <t>Ocai 'black/smoke grey'</t>
+  </si>
+  <si>
+    <t>DC Shoes Court Graffik White</t>
+  </si>
+  <si>
+    <t>Campus x bad bunny 'black'</t>
+  </si>
+  <si>
+    <t>Nike Air Huarache Craft 'Smokey Grey'</t>
+  </si>
+  <si>
+    <t>Nike Air Jordan 1 Low x Travis Scott 'Tiffany'</t>
+  </si>
+  <si>
+    <t>Campus 00s 'Ambient Sky'</t>
+  </si>
+  <si>
+    <t>Campus 00s 'Grey'</t>
+  </si>
+  <si>
+    <t>Nike Zoom Vomero 5 'Oatmeal'</t>
+  </si>
+  <si>
+    <t>Response x Bad Bunny CL 'Cream White'</t>
+  </si>
+  <si>
+    <t>A BATHING APE Bape Sta Hi 'black/white'</t>
+  </si>
+  <si>
+    <t>ADI2000 'Lab Green'</t>
+  </si>
+  <si>
+    <t>Forum 84 Low 'Off white'</t>
+  </si>
+  <si>
+    <t>Nike Dunk Low Pro SB 'Thunderstorm'</t>
+  </si>
+  <si>
+    <t>Nike Dunk Low 'Dusty Olive'</t>
+  </si>
+  <si>
+    <t>Nike LPL X Dunk Low 'Black White Red'</t>
   </si>
   <si>
     <t>Saucony Jazz 'Grey/Black' New</t>
-  </si>
-  <si>
-    <t>Nike Air Max 90 Terrascape 'Sail Sea Glass'</t>
-  </si>
-  <si>
-    <t>Nike X Grateful Dead SB Dunk Low 'Orange Bear'</t>
-  </si>
-  <si>
-    <t>Niteball 'Black Sub Green'</t>
-  </si>
-  <si>
-    <t>Nike Air Jordan 4 Retro SE 'Neon 95'</t>
-  </si>
-  <si>
-    <t>Superstar 'White/Black'</t>
-  </si>
-  <si>
-    <t>Merrell ice cap moc 'black/orange'</t>
-  </si>
-  <si>
-    <t>ASICS Gel-NYC 'Mauve Blue'</t>
-  </si>
-  <si>
-    <t>Nike Air Max 95 'Koi'</t>
-  </si>
-  <si>
-    <t>Nike x Supreme Shox Ride 2 SP White/Grey/Volt</t>
-  </si>
-  <si>
-    <t>Nike Air Max 95 Petek 'Dark Blue/Purple'</t>
-  </si>
-  <si>
-    <t>Nike Air Max 95 white/black/fiol</t>
-  </si>
-  <si>
-    <t>Nike Shox Ride 2 'Baroque Brown Diffused Blue</t>
-  </si>
-  <si>
-    <t>Nike Shox TL 'Persian Violet'</t>
-  </si>
-  <si>
-    <t>Nike Nocta Glide Drake 'Khaki'</t>
-  </si>
-  <si>
-    <t>Nike Air Max Portal 'Black/White'</t>
-  </si>
-  <si>
-    <t>Nike Air Max 96 'Triple Black'</t>
-  </si>
-  <si>
-    <t>Nike Air Force low 'Venom'</t>
-  </si>
-  <si>
-    <t>Nike Dunk Low 'Year of the Dragon'</t>
-  </si>
-  <si>
-    <t>Nike Kyrie 7 EP 'Chinese New Year'</t>
-  </si>
-  <si>
-    <t>Asics Gel-NYC Gore-Tex 'Black/Bronze'</t>
-  </si>
-  <si>
-    <t>Salomon XT-6 GORE-TEX  'Triple Black'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ASICS Gel Kayano Trainer 21 'Black' </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SALOMON XT-6 'Pewter Black Aurora Red' </t>
-  </si>
-  <si>
-    <t>Nike Dunk Low 'Sanddrift Light Armory Blue'</t>
-  </si>
-  <si>
-    <t>Nike Air Jordan 4 retro 'military brown'</t>
-  </si>
-  <si>
-    <t>ASICS Gel-Kayano Trainer 21 'Smoke Blue'</t>
-  </si>
-  <si>
-    <t>Nike Air Max Terrascape Plus 'Triple Black'</t>
-  </si>
-  <si>
-    <t>Salomon XT-6 Series 'Black/Lunar Rock'</t>
-  </si>
-  <si>
-    <t>Globe Tilt trainers 'Dark Shadow/Phantom'</t>
-  </si>
-  <si>
-    <t>DC Shoes Spectre x NEEDLES 'Black/Purple'</t>
-  </si>
-  <si>
-    <t>Iniki Runner 'Core Black 2.0'</t>
-  </si>
-  <si>
-    <t>ASICS Gel 1090 'Silver'</t>
-  </si>
-  <si>
-    <t>Nike Air Zoom Pegasus 38 'Wolf Grey'</t>
-  </si>
-  <si>
-    <t>Nike Zoom Pegasus 39 'Ashen Slate Football Grey Cobalt Bliss'</t>
-  </si>
-  <si>
-    <t>Nike ZoomX Zegama Trail 2 'Black/White'</t>
-  </si>
-  <si>
-    <t>ASICS GEL-1130 X HAL STUDIOS 'Smoke Grey'</t>
-  </si>
-  <si>
-    <t>Nike v2k run 'metallic silver/white'</t>
-  </si>
-  <si>
-    <t>Asics Gel-1130 'Slate Grey/Piedmont Grey'</t>
-  </si>
-  <si>
-    <t>Asics gel-1130 X HAL STUDIOS  'Forest'</t>
-  </si>
-  <si>
-    <t>Suba Sport black red</t>
-  </si>
-  <si>
-    <t>Intimidation Sports Casual Shoes 'Black Purple'</t>
-  </si>
-  <si>
-    <t>Premiata Mick 'Black'</t>
-  </si>
-  <si>
-    <t>Nike SB Dunk Low Vintage 'Phoenix Suns'</t>
-  </si>
-  <si>
-    <t>ASICS GEL SONOMA 15 White/Dark grey</t>
-  </si>
-  <si>
-    <t>Saucony Jazz Original Vintage 'Light Grey'</t>
-  </si>
-  <si>
-    <t>ASICS Gel-Kahana 8 'Dark Blue Brown' demi</t>
-  </si>
-  <si>
-    <t>Zig Kinetica 2 Edge GTX 'Black'</t>
-  </si>
-  <si>
-    <t>Salomon XT-6 'Triple Black'</t>
-  </si>
-  <si>
-    <t>Nike Air Jordan MVP 678 'Raptors'</t>
-  </si>
-  <si>
-    <t>Nike Air Jordan 6 Retro x Travis Scott 'Olive'</t>
-  </si>
-  <si>
-    <t>Nike SB Dunk Low х Stussy 'BMW M3'</t>
-  </si>
-  <si>
-    <t>Ocai 'black/smoke grey'</t>
-  </si>
-  <si>
-    <t>DC Shoes Court Graffik White</t>
-  </si>
-  <si>
-    <t>Campus x bad bunny 'black'</t>
-  </si>
-  <si>
-    <t>Nike Air Huarache Craft 'Smokey Grey'</t>
-  </si>
-  <si>
-    <t>Nike Air Jordan 1 Low x Travis Scott 'Tiffany'</t>
-  </si>
-  <si>
-    <t>Campus 00s 'Ambient Sky'</t>
-  </si>
-  <si>
-    <t>Campus 00s 'Grey'</t>
-  </si>
-  <si>
-    <t>Nike Zoom Vomero 5 'Oatmeal'</t>
-  </si>
-  <si>
-    <t>Response x Bad Bunny CL 'Cream White'</t>
-  </si>
-  <si>
-    <t>A BATHING APE Bape Sta Hi 'black/white'</t>
-  </si>
-  <si>
-    <t>ADI2000 'Lab Green'</t>
-  </si>
-  <si>
-    <t>Forum 84 Low 'Off white'</t>
-  </si>
-  <si>
-    <t>Nike Dunk Low Pro SB 'Thunderstorm'</t>
-  </si>
-  <si>
-    <t>Nike Dunk Low 'Dusty Olive'</t>
-  </si>
-  <si>
-    <t>Nike LPL X Dunk Low 'Black White Red'</t>
   </si>
   <si>
     <t>Nike Air Max 96 'Beach'</t>
@@ -1695,7 +1695,7 @@
         <v>66</v>
       </c>
       <c r="B67">
-        <v>130</v>
+        <v>135</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -1727,7 +1727,7 @@
         <v>70</v>
       </c>
       <c r="B71">
-        <v>135</v>
+        <v>95</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -1759,7 +1759,7 @@
         <v>74</v>
       </c>
       <c r="B75">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -1767,7 +1767,7 @@
         <v>75</v>
       </c>
       <c r="B76">
-        <v>85</v>
+        <v>100</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -1775,7 +1775,7 @@
         <v>76</v>
       </c>
       <c r="B77">
-        <v>100</v>
+        <v>150</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -1783,7 +1783,7 @@
         <v>77</v>
       </c>
       <c r="B78">
-        <v>150</v>
+        <v>95</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -1799,7 +1799,7 @@
         <v>79</v>
       </c>
       <c r="B80">
-        <v>95</v>
+        <v>130</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -1807,7 +1807,7 @@
         <v>80</v>
       </c>
       <c r="B81">
-        <v>130</v>
+        <v>135</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -1823,7 +1823,7 @@
         <v>82</v>
       </c>
       <c r="B83">
-        <v>135</v>
+        <v>95</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -1839,7 +1839,7 @@
         <v>84</v>
       </c>
       <c r="B85">
-        <v>95</v>
+        <v>135</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -1847,7 +1847,7 @@
         <v>85</v>
       </c>
       <c r="B86">
-        <v>135</v>
+        <v>150</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -1871,7 +1871,7 @@
         <v>88</v>
       </c>
       <c r="B89">
-        <v>150</v>
+        <v>75</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -1879,7 +1879,7 @@
         <v>89</v>
       </c>
       <c r="B90">
-        <v>75</v>
+        <v>150</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -1887,7 +1887,7 @@
         <v>90</v>
       </c>
       <c r="B91">
-        <v>150</v>
+        <v>120</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -1895,7 +1895,7 @@
         <v>91</v>
       </c>
       <c r="B92">
-        <v>120</v>
+        <v>95</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -1903,7 +1903,7 @@
         <v>92</v>
       </c>
       <c r="B93">
-        <v>95</v>
+        <v>65</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -1911,7 +1911,7 @@
         <v>93</v>
       </c>
       <c r="B94">
-        <v>65</v>
+        <v>150</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -1919,7 +1919,7 @@
         <v>94</v>
       </c>
       <c r="B95">
-        <v>150</v>
+        <v>120</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -1951,7 +1951,7 @@
         <v>98</v>
       </c>
       <c r="B99">
-        <v>120</v>
+        <v>95</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -1959,7 +1959,7 @@
         <v>99</v>
       </c>
       <c r="B100">
-        <v>95</v>
+        <v>135</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -1975,7 +1975,7 @@
         <v>101</v>
       </c>
       <c r="B102">
-        <v>135</v>
+        <v>150</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -1991,7 +1991,7 @@
         <v>103</v>
       </c>
       <c r="B104">
-        <v>150</v>
+        <v>130</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -2303,7 +2303,7 @@
         <v>142</v>
       </c>
       <c r="B143">
-        <v>130</v>
+        <v>95</v>
       </c>
     </row>
     <row r="144" spans="1:2">
@@ -2311,7 +2311,7 @@
         <v>143</v>
       </c>
       <c r="B144">
-        <v>95</v>
+        <v>130</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -2319,7 +2319,7 @@
         <v>144</v>
       </c>
       <c r="B145">
-        <v>130</v>
+        <v>150</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -2327,7 +2327,7 @@
         <v>145</v>
       </c>
       <c r="B146">
-        <v>150</v>
+        <v>75</v>
       </c>
     </row>
     <row r="147" spans="1:2">
@@ -2335,7 +2335,7 @@
         <v>146</v>
       </c>
       <c r="B147">
-        <v>75</v>
+        <v>130</v>
       </c>
     </row>
     <row r="148" spans="1:2">
@@ -2343,7 +2343,7 @@
         <v>147</v>
       </c>
       <c r="B148">
-        <v>130</v>
+        <v>140</v>
       </c>
     </row>
     <row r="149" spans="1:2">
@@ -2351,7 +2351,7 @@
         <v>148</v>
       </c>
       <c r="B149">
-        <v>120</v>
+        <v>130</v>
       </c>
     </row>
     <row r="150" spans="1:2">
@@ -2359,7 +2359,7 @@
         <v>149</v>
       </c>
       <c r="B150">
-        <v>140</v>
+        <v>120</v>
       </c>
     </row>
     <row r="151" spans="1:2">
@@ -2367,7 +2367,7 @@
         <v>150</v>
       </c>
       <c r="B151">
-        <v>130</v>
+        <v>140</v>
       </c>
     </row>
     <row r="152" spans="1:2">
@@ -2375,7 +2375,7 @@
         <v>151</v>
       </c>
       <c r="B152">
-        <v>120</v>
+        <v>150</v>
       </c>
     </row>
     <row r="153" spans="1:2">
@@ -2383,7 +2383,7 @@
         <v>152</v>
       </c>
       <c r="B153">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="154" spans="1:2">
@@ -2391,7 +2391,7 @@
         <v>153</v>
       </c>
       <c r="B154">
-        <v>150</v>
+        <v>95</v>
       </c>
     </row>
     <row r="155" spans="1:2">
@@ -2399,7 +2399,7 @@
         <v>154</v>
       </c>
       <c r="B155">
-        <v>135</v>
+        <v>95</v>
       </c>
     </row>
     <row r="156" spans="1:2">
@@ -2407,7 +2407,7 @@
         <v>155</v>
       </c>
       <c r="B156">
-        <v>95</v>
+        <v>75</v>
       </c>
     </row>
     <row r="157" spans="1:2">
@@ -2423,7 +2423,7 @@
         <v>157</v>
       </c>
       <c r="B158">
-        <v>75</v>
+        <v>150</v>
       </c>
     </row>
     <row r="159" spans="1:2">
@@ -2431,7 +2431,7 @@
         <v>158</v>
       </c>
       <c r="B159">
-        <v>95</v>
+        <v>65</v>
       </c>
     </row>
     <row r="160" spans="1:2">
@@ -2439,7 +2439,7 @@
         <v>159</v>
       </c>
       <c r="B160">
-        <v>150</v>
+        <v>140</v>
       </c>
     </row>
     <row r="161" spans="1:2">
@@ -2447,7 +2447,7 @@
         <v>160</v>
       </c>
       <c r="B161">
-        <v>65</v>
+        <v>135</v>
       </c>
     </row>
     <row r="162" spans="1:2">
@@ -2455,7 +2455,7 @@
         <v>161</v>
       </c>
       <c r="B162">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="163" spans="1:2">
@@ -2463,7 +2463,7 @@
         <v>162</v>
       </c>
       <c r="B163">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="164" spans="1:2">
@@ -2471,7 +2471,7 @@
         <v>163</v>
       </c>
       <c r="B164">
-        <v>135</v>
+        <v>120</v>
       </c>
     </row>
     <row r="165" spans="1:2">
@@ -2479,7 +2479,7 @@
         <v>164</v>
       </c>
       <c r="B165">
-        <v>130</v>
+        <v>120</v>
       </c>
     </row>
     <row r="166" spans="1:2">
@@ -2487,7 +2487,7 @@
         <v>165</v>
       </c>
       <c r="B166">
-        <v>120</v>
+        <v>130</v>
       </c>
     </row>
     <row r="167" spans="1:2">
@@ -2495,7 +2495,7 @@
         <v>166</v>
       </c>
       <c r="B167">
-        <v>120</v>
+        <v>130</v>
       </c>
     </row>
     <row r="168" spans="1:2">
@@ -2503,7 +2503,7 @@
         <v>167</v>
       </c>
       <c r="B168">
-        <v>130</v>
+        <v>120</v>
       </c>
     </row>
     <row r="169" spans="1:2">
@@ -2511,7 +2511,7 @@
         <v>168</v>
       </c>
       <c r="B169">
-        <v>130</v>
+        <v>95</v>
       </c>
     </row>
     <row r="170" spans="1:2">
@@ -2519,7 +2519,7 @@
         <v>169</v>
       </c>
       <c r="B170">
-        <v>120</v>
+        <v>95</v>
       </c>
     </row>
     <row r="171" spans="1:2">
@@ -2527,7 +2527,7 @@
         <v>170</v>
       </c>
       <c r="B171">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="172" spans="1:2">
@@ -2535,7 +2535,7 @@
         <v>171</v>
       </c>
       <c r="B172">
-        <v>95</v>
+        <v>65</v>
       </c>
     </row>
     <row r="173" spans="1:2">
@@ -2543,7 +2543,7 @@
         <v>172</v>
       </c>
       <c r="B173">
-        <v>85</v>
+        <v>135</v>
       </c>
     </row>
     <row r="174" spans="1:2">
@@ -2551,7 +2551,7 @@
         <v>173</v>
       </c>
       <c r="B174">
-        <v>65</v>
+        <v>130</v>
       </c>
     </row>
     <row r="175" spans="1:2">
@@ -2559,7 +2559,7 @@
         <v>174</v>
       </c>
       <c r="B175">
-        <v>135</v>
+        <v>120</v>
       </c>
     </row>
     <row r="176" spans="1:2">
@@ -2567,7 +2567,7 @@
         <v>175</v>
       </c>
       <c r="B176">
-        <v>130</v>
+        <v>75</v>
       </c>
     </row>
     <row r="177" spans="1:2">
@@ -2583,7 +2583,7 @@
         <v>177</v>
       </c>
       <c r="B178">
-        <v>75</v>
+        <v>130</v>
       </c>
     </row>
     <row r="179" spans="1:2">
@@ -2591,7 +2591,7 @@
         <v>178</v>
       </c>
       <c r="B179">
-        <v>120</v>
+        <v>150</v>
       </c>
     </row>
     <row r="180" spans="1:2">
@@ -2599,7 +2599,7 @@
         <v>179</v>
       </c>
       <c r="B180">
-        <v>130</v>
+        <v>65</v>
       </c>
     </row>
     <row r="181" spans="1:2">
@@ -2623,7 +2623,7 @@
         <v>182</v>
       </c>
       <c r="B183">
-        <v>150</v>
+        <v>95</v>
       </c>
     </row>
     <row r="184" spans="1:2">
@@ -2631,7 +2631,7 @@
         <v>183</v>
       </c>
       <c r="B184">
-        <v>65</v>
+        <v>75</v>
       </c>
     </row>
     <row r="185" spans="1:2">
@@ -2639,7 +2639,7 @@
         <v>184</v>
       </c>
       <c r="B185">
-        <v>95</v>
+        <v>65</v>
       </c>
     </row>
     <row r="186" spans="1:2">
@@ -2647,7 +2647,7 @@
         <v>185</v>
       </c>
       <c r="B186">
-        <v>95</v>
+        <v>65</v>
       </c>
     </row>
     <row r="187" spans="1:2">
@@ -2655,7 +2655,7 @@
         <v>186</v>
       </c>
       <c r="B187">
-        <v>75</v>
+        <v>135</v>
       </c>
     </row>
     <row r="188" spans="1:2">
@@ -2663,7 +2663,7 @@
         <v>187</v>
       </c>
       <c r="B188">
-        <v>65</v>
+        <v>100</v>
       </c>
     </row>
     <row r="189" spans="1:2">
@@ -2671,7 +2671,7 @@
         <v>188</v>
       </c>
       <c r="B189">
-        <v>65</v>
+        <v>140</v>
       </c>
     </row>
     <row r="190" spans="1:2">
@@ -2679,7 +2679,7 @@
         <v>189</v>
       </c>
       <c r="B190">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="191" spans="1:2">
@@ -2687,7 +2687,7 @@
         <v>190</v>
       </c>
       <c r="B191">
-        <v>100</v>
+        <v>130</v>
       </c>
     </row>
     <row r="192" spans="1:2">
@@ -2695,7 +2695,7 @@
         <v>191</v>
       </c>
       <c r="B192">
-        <v>140</v>
+        <v>150</v>
       </c>
     </row>
     <row r="193" spans="1:2">
@@ -2711,7 +2711,7 @@
         <v>193</v>
       </c>
       <c r="B194">
-        <v>150</v>
+        <v>130</v>
       </c>
     </row>
     <row r="195" spans="1:2">
@@ -2719,7 +2719,7 @@
         <v>194</v>
       </c>
       <c r="B195">
-        <v>130</v>
+        <v>150</v>
       </c>
     </row>
     <row r="196" spans="1:2">
@@ -2727,7 +2727,7 @@
         <v>195</v>
       </c>
       <c r="B196">
-        <v>130</v>
+        <v>150</v>
       </c>
     </row>
     <row r="197" spans="1:2">
@@ -2735,7 +2735,7 @@
         <v>196</v>
       </c>
       <c r="B197">
-        <v>150</v>
+        <v>140</v>
       </c>
     </row>
     <row r="198" spans="1:2">
@@ -2743,7 +2743,7 @@
         <v>197</v>
       </c>
       <c r="B198">
-        <v>150</v>
+        <v>120</v>
       </c>
     </row>
     <row r="199" spans="1:2">
@@ -2751,7 +2751,7 @@
         <v>198</v>
       </c>
       <c r="B199">
-        <v>140</v>
+        <v>120</v>
       </c>
     </row>
     <row r="200" spans="1:2">
@@ -2759,7 +2759,7 @@
         <v>199</v>
       </c>
       <c r="B200">
-        <v>120</v>
+        <v>150</v>
       </c>
     </row>
     <row r="201" spans="1:2">
@@ -2767,7 +2767,7 @@
         <v>200</v>
       </c>
       <c r="B201">
-        <v>150</v>
+        <v>120</v>
       </c>
     </row>
     <row r="202" spans="1:2">
@@ -2775,7 +2775,7 @@
         <v>201</v>
       </c>
       <c r="B202">
-        <v>120</v>
+        <v>95</v>
       </c>
     </row>
     <row r="203" spans="1:2">
@@ -2807,7 +2807,7 @@
         <v>205</v>
       </c>
       <c r="B206">
-        <v>95</v>
+        <v>140</v>
       </c>
     </row>
     <row r="207" spans="1:2">
@@ -2815,7 +2815,7 @@
         <v>206</v>
       </c>
       <c r="B207">
-        <v>140</v>
+        <v>95</v>
       </c>
     </row>
     <row r="208" spans="1:2">
@@ -2831,7 +2831,7 @@
         <v>208</v>
       </c>
       <c r="B209">
-        <v>95</v>
+        <v>65</v>
       </c>
     </row>
     <row r="210" spans="1:2">
@@ -2839,7 +2839,7 @@
         <v>209</v>
       </c>
       <c r="B210">
-        <v>65</v>
+        <v>140</v>
       </c>
     </row>
     <row r="211" spans="1:2">
@@ -2847,7 +2847,7 @@
         <v>210</v>
       </c>
       <c r="B211">
-        <v>140</v>
+        <v>95</v>
       </c>
     </row>
     <row r="212" spans="1:2">
@@ -2863,7 +2863,7 @@
         <v>212</v>
       </c>
       <c r="B213">
-        <v>95</v>
+        <v>150</v>
       </c>
     </row>
     <row r="214" spans="1:2">
@@ -2871,7 +2871,7 @@
         <v>213</v>
       </c>
       <c r="B214">
-        <v>150</v>
+        <v>95</v>
       </c>
     </row>
     <row r="215" spans="1:2">
@@ -2879,7 +2879,7 @@
         <v>214</v>
       </c>
       <c r="B215">
-        <v>95</v>
+        <v>125</v>
       </c>
     </row>
     <row r="216" spans="1:2">
@@ -2887,7 +2887,7 @@
         <v>215</v>
       </c>
       <c r="B216">
-        <v>125</v>
+        <v>140</v>
       </c>
     </row>
     <row r="217" spans="1:2">
@@ -2895,7 +2895,7 @@
         <v>216</v>
       </c>
       <c r="B217">
-        <v>140</v>
+        <v>120</v>
       </c>
     </row>
     <row r="218" spans="1:2">
@@ -2919,7 +2919,7 @@
         <v>219</v>
       </c>
       <c r="B220">
-        <v>120</v>
+        <v>140</v>
       </c>
     </row>
     <row r="221" spans="1:2">
@@ -2951,7 +2951,7 @@
         <v>223</v>
       </c>
       <c r="B224">
-        <v>140</v>
+        <v>50</v>
       </c>
     </row>
     <row r="225" spans="1:2">
@@ -2959,7 +2959,7 @@
         <v>224</v>
       </c>
       <c r="B225">
-        <v>50</v>
+        <v>140</v>
       </c>
     </row>
     <row r="226" spans="1:2">
@@ -2975,7 +2975,7 @@
         <v>226</v>
       </c>
       <c r="B227">
-        <v>140</v>
+        <v>95</v>
       </c>
     </row>
     <row r="228" spans="1:2">
@@ -2983,7 +2983,7 @@
         <v>227</v>
       </c>
       <c r="B228">
-        <v>95</v>
+        <v>140</v>
       </c>
     </row>
     <row r="229" spans="1:2">
@@ -2991,7 +2991,7 @@
         <v>228</v>
       </c>
       <c r="B229">
-        <v>140</v>
+        <v>150</v>
       </c>
     </row>
     <row r="230" spans="1:2">
@@ -3007,7 +3007,7 @@
         <v>230</v>
       </c>
       <c r="B231">
-        <v>150</v>
+        <v>100</v>
       </c>
     </row>
     <row r="232" spans="1:2">
@@ -3015,7 +3015,7 @@
         <v>231</v>
       </c>
       <c r="B232">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="233" spans="1:2">
@@ -3031,7 +3031,7 @@
         <v>233</v>
       </c>
       <c r="B234">
-        <v>95</v>
+        <v>110</v>
       </c>
     </row>
     <row r="235" spans="1:2">
@@ -3039,7 +3039,7 @@
         <v>234</v>
       </c>
       <c r="B235">
-        <v>110</v>
+        <v>95</v>
       </c>
     </row>
     <row r="236" spans="1:2">
@@ -3047,7 +3047,7 @@
         <v>235</v>
       </c>
       <c r="B236">
-        <v>95</v>
+        <v>110</v>
       </c>
     </row>
     <row r="237" spans="1:2">
@@ -3055,7 +3055,7 @@
         <v>236</v>
       </c>
       <c r="B237">
-        <v>110</v>
+        <v>95</v>
       </c>
     </row>
     <row r="238" spans="1:2">
@@ -3079,7 +3079,7 @@
         <v>239</v>
       </c>
       <c r="B240">
-        <v>95</v>
+        <v>75</v>
       </c>
     </row>
     <row r="241" spans="1:2">
@@ -3103,7 +3103,7 @@
         <v>242</v>
       </c>
       <c r="B243">
-        <v>75</v>
+        <v>140</v>
       </c>
     </row>
     <row r="244" spans="1:2">
@@ -3119,7 +3119,7 @@
         <v>244</v>
       </c>
       <c r="B245">
-        <v>140</v>
+        <v>65</v>
       </c>
     </row>
     <row r="246" spans="1:2">
@@ -3135,7 +3135,7 @@
         <v>246</v>
       </c>
       <c r="B247">
-        <v>65</v>
+        <v>95</v>
       </c>
     </row>
     <row r="248" spans="1:2">
@@ -3143,7 +3143,7 @@
         <v>247</v>
       </c>
       <c r="B248">
-        <v>95</v>
+        <v>75</v>
       </c>
     </row>
     <row r="249" spans="1:2">
@@ -3151,7 +3151,7 @@
         <v>248</v>
       </c>
       <c r="B249">
-        <v>75</v>
+        <v>95</v>
       </c>
     </row>
     <row r="250" spans="1:2">
@@ -3159,7 +3159,7 @@
         <v>249</v>
       </c>
       <c r="B250">
-        <v>95</v>
+        <v>75</v>
       </c>
     </row>
     <row r="251" spans="1:2">
@@ -3167,7 +3167,7 @@
         <v>250</v>
       </c>
       <c r="B251">
-        <v>75</v>
+        <v>95</v>
       </c>
     </row>
     <row r="252" spans="1:2">

</xml_diff>